<commit_message>
loading and downloading world & code files, some refactoring
</commit_message>
<xml_diff>
--- a/WorldBuilder.xlsx
+++ b/WorldBuilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0857f1007b00f174/Desktop/CodeProjects/RK4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{B216423E-515C-46F0-8485-44DA8BD5A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{836BBE34-4820-417E-9B24-C23850D64AE4}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{B216423E-515C-46F0-8485-44DA8BD5A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEC6307A-E6C5-4BE8-BF41-8FA26F5DA721}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{552B6719-560E-4CE6-9C46-D2BB944E1FD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{552B6719-560E-4CE6-9C46-D2BB944E1FD4}"/>
   </bookViews>
   <sheets>
     <sheet name="WorldBuilder" sheetId="1" r:id="rId1"/>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF99E9F-59C5-4BC8-8BBC-57EB6CF50C05}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>2</v>
@@ -930,7 +930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A378B9-FFC7-414F-922C-D24122462C01}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>